<commit_message>
examiner comments part 1
</commit_message>
<xml_diff>
--- a/tables/Ch1-austickmicrobes.xlsx
+++ b/tables/Ch1-austickmicrobes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Siobhon/Documents/Uni/PhD/Thesis-docs/PhD/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34BA902-FA07-6B42-B0FD-27B12B6CE42F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97559F1-3869-A24B-A1BA-A89C4BA0C584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{3F5E57B6-4799-694D-AB9A-271590BD3E2C}"/>
+    <workbookView xWindow="1040" yWindow="460" windowWidth="21340" windowHeight="17540" xr2:uid="{3F5E57B6-4799-694D-AB9A-271590BD3E2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1937" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1949" uniqueCount="434">
   <si>
     <t>Tick species</t>
   </si>
@@ -1648,6 +1648,39 @@
   </si>
   <si>
     <t>Krige et al. 2021</t>
+  </si>
+  <si>
+    <t>Bt. concolor, Ha. Humerosa</t>
+  </si>
+  <si>
+    <t>Am. Albolimbatum</t>
+  </si>
+  <si>
+    <t>Angus 1996; Jonsson et al. 2008</t>
+  </si>
+  <si>
+    <t>NSW, QLD, WA</t>
+  </si>
+  <si>
+    <t>Babesia bigemina (a)</t>
+  </si>
+  <si>
+    <t>Babesia bovis (a)</t>
+  </si>
+  <si>
+    <t>Coxiella burnetii</t>
+  </si>
+  <si>
+    <t>Coxiella burnetii (a)</t>
+  </si>
+  <si>
+    <t>‘Ca. Ehrlichia occidentalis’</t>
+  </si>
+  <si>
+    <t>‘Ca. Ehrlichia ornithorhynchi’</t>
+  </si>
+  <si>
+    <t>Ehrlichia sp.</t>
   </si>
 </sst>
 </file>
@@ -2079,10 +2112,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA96E089-1365-8248-A283-2AF976655E18}">
-  <dimension ref="A1:F107"/>
+  <dimension ref="A1:F109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="F106" sqref="F106"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2091,7 +2124,7 @@
     <col min="2" max="2" width="18.33203125" style="5" customWidth="1"/>
     <col min="3" max="3" width="25" style="5" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="5"/>
-    <col min="5" max="5" width="9" style="5" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.5" style="5" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="5"/>
   </cols>
@@ -2357,7 +2390,7 @@
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -2381,7 +2414,7 @@
         <v>107</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>108</v>
+        <v>424</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>109</v>
@@ -2398,7 +2431,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2" t="s">
-        <v>70</v>
+        <v>429</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>41</v>
@@ -2418,7 +2451,7 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
-        <v>70</v>
+        <v>429</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>83</v>
@@ -2438,7 +2471,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
-        <v>70</v>
+        <v>429</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>84</v>
@@ -2458,7 +2491,7 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>337</v>
+        <v>430</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>85</v>
@@ -2478,7 +2511,7 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
-        <v>70</v>
+        <v>429</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>83</v>
@@ -2498,7 +2531,7 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2" t="s">
-        <v>70</v>
+        <v>429</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>86</v>
@@ -2518,7 +2551,7 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2" t="s">
-        <v>70</v>
+        <v>429</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>39</v>
@@ -2538,7 +2571,7 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2" t="s">
-        <v>70</v>
+        <v>429</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>83</v>
@@ -2658,13 +2691,13 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="4" t="s">
-        <v>50</v>
+        <v>431</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>55</v>
+        <v>280</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>6</v>
@@ -2678,7 +2711,7 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="4" t="s">
-        <v>49</v>
+        <v>432</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>54</v>
@@ -2704,7 +2737,7 @@
         <v>35</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>55</v>
+        <v>280</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>6</v>
@@ -2718,7 +2751,7 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="2" t="s">
-        <v>52</v>
+        <v>433</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>57</v>
@@ -2881,7 +2914,7 @@
         <v>106</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>246</v>
+        <v>423</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>350</v>
@@ -3637,114 +3670,114 @@
       </c>
     </row>
     <row r="78" spans="1:6">
-      <c r="A78" s="8" t="s">
+      <c r="A78" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B80" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C78" s="8" t="s">
+      <c r="C80" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="D80" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="E78" s="5" t="s">
+      <c r="E80" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="F78" s="5" t="s">
+      <c r="F80" s="5" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
-      <c r="A79" s="8" t="s">
+    <row r="81" spans="1:6">
+      <c r="A81" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B81" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C79" s="8" t="s">
+      <c r="C81" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="D79" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E79" s="5" t="s">
+      <c r="D81" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E81" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F79" s="5" t="s">
+      <c r="F81" s="5" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
-      <c r="A80" s="5" t="s">
+    <row r="82" spans="1:6">
+      <c r="A82" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B82" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C80" s="8" t="s">
+      <c r="C82" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="D80" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E80" s="5" t="s">
+      <c r="D82" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E82" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F80" s="5" t="s">
+      <c r="F82" s="5" t="s">
         <v>259</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
-      <c r="A81" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E81" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F81" s="5" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
-      <c r="A82" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="C82" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D82" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E82" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="5" t="s">
-        <v>340</v>
+        <v>308</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>6</v>
@@ -3757,148 +3790,148 @@
       </c>
     </row>
     <row r="84" spans="1:6">
-      <c r="A84" s="5" t="s">
+      <c r="A84" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="5" t="s">
         <v>340</v>
       </c>
-      <c r="B84" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="D84" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E84" s="5" t="s">
+      <c r="B85" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E85" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F84" s="5" t="s">
+      <c r="F85" s="5" t="s">
         <v>265</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
-      <c r="A85" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="B85" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C85" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E85" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="B86" s="8" t="s">
+      <c r="B88" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="C86" s="8" t="s">
+      <c r="C88" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="D86" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E86" s="5" t="s">
+      <c r="D88" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E88" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F86" s="5" t="s">
+      <c r="F88" s="5" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
-      <c r="A87" s="8" t="s">
+    <row r="89" spans="1:6">
+      <c r="A89" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="B87" s="8" t="s">
+      <c r="B89" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="C87" s="8" t="s">
+      <c r="C89" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="D87" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E87" s="5" t="s">
+      <c r="D89" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E89" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F87" s="5" t="s">
+      <c r="F89" s="5" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
-      <c r="A88" s="8" t="s">
+    <row r="90" spans="1:6">
+      <c r="A90" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="B88" s="8" t="s">
+      <c r="B90" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C88" s="8" t="s">
+      <c r="C90" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="D90" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
-      <c r="A89" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="B89" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C89" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D89" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6">
-      <c r="A90" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="B90" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C90" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>6</v>
       </c>
       <c r="E90" s="5" t="s">
         <v>19</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>417</v>
+        <v>274</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B91" s="8" t="s">
         <v>37</v>
@@ -3917,74 +3950,74 @@
       </c>
     </row>
     <row r="92" spans="1:6">
-      <c r="A92" s="5" t="s">
-        <v>290</v>
+      <c r="A92" s="2" t="s">
+        <v>249</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D92" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>259</v>
+        <v>417</v>
       </c>
     </row>
     <row r="93" spans="1:6">
-      <c r="A93" s="5" t="s">
+      <c r="A93" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F93" s="5" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="5" t="s">
         <v>290</v>
-      </c>
-      <c r="B93" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="C93" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="D93" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E93" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F93" s="5" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6">
-      <c r="A94" s="8" t="s">
-        <v>261</v>
       </c>
       <c r="B94" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="D94" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="95" spans="1:6">
-      <c r="A95" s="8" t="s">
-        <v>261</v>
+      <c r="A95" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>22</v>
+        <v>264</v>
       </c>
       <c r="D95" s="5" t="s">
         <v>6</v>
@@ -3998,102 +4031,102 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="8" t="s">
-        <v>285</v>
+        <v>261</v>
       </c>
       <c r="B96" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D96" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>417</v>
+        <v>265</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" s="8" t="s">
-        <v>358</v>
+        <v>261</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>9</v>
+        <v>122</v>
       </c>
       <c r="F97" s="5" t="s">
-        <v>416</v>
+        <v>265</v>
       </c>
     </row>
     <row r="98" spans="1:6">
       <c r="A98" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D98" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>122</v>
+        <v>19</v>
       </c>
       <c r="F98" s="5" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="99" spans="1:6">
-      <c r="A99" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="B99" s="5" t="s">
-        <v>359</v>
+      <c r="A99" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>360</v>
+        <v>56</v>
       </c>
       <c r="D99" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="100" spans="1:6">
-      <c r="A100" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>361</v>
+      <c r="A100" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>360</v>
+        <v>31</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>64</v>
+        <v>122</v>
       </c>
       <c r="F100" s="5" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -4101,70 +4134,70 @@
         <v>344</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>37</v>
+        <v>359</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>18</v>
+        <v>360</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="102" spans="1:6">
-      <c r="A102" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="B102" s="8" t="s">
-        <v>276</v>
+      <c r="A102" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>361</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D102" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>372</v>
+        <v>415</v>
       </c>
     </row>
     <row r="103" spans="1:6">
-      <c r="A103" s="8" t="s">
-        <v>309</v>
-      </c>
-      <c r="B103" s="8" t="s">
-        <v>42</v>
+      <c r="A103" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="F103" s="5" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" s="8" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>37</v>
+        <v>276</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>46</v>
+        <v>362</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>4</v>
@@ -4173,32 +4206,32 @@
         <v>61</v>
       </c>
       <c r="F104" s="5" t="s">
-        <v>421</v>
+        <v>372</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" s="8" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>280</v>
+        <v>46</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>281</v>
+        <v>4</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="F105" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" s="8" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B106" s="8" t="s">
         <v>37</v>
@@ -4213,26 +4246,66 @@
         <v>61</v>
       </c>
       <c r="F106" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="B107" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C107" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="B108" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C108" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E108" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F108" s="5" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
-      <c r="A107" s="5" t="s">
+    <row r="109" spans="1:6">
+      <c r="A109" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="B107" s="5" t="s">
+      <c r="B109" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C107" s="8" t="s">
+      <c r="C109" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D107" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E107" s="5" t="s">
+      <c r="D109" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E109" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F107" s="5" t="s">
+      <c r="F109" s="5" t="s">
         <v>306</v>
       </c>
     </row>

</xml_diff>